<commit_message>
added changing words on demand
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="363">
   <si>
     <t>Rodzaj</t>
   </si>
@@ -1089,10 +1089,16 @@
     <t>łazienka</t>
   </si>
   <si>
+    <t>ett badrum</t>
+  </si>
+  <si>
+    <t>lodowka</t>
+  </si>
+  <si>
+    <t>ett kylskåp</t>
+  </si>
+  <si>
     <t>badrum</t>
-  </si>
-  <si>
-    <t>lodowka</t>
   </si>
   <si>
     <t>kylskåp</t>
@@ -7460,7 +7466,7 @@
         <v>357</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="179">
@@ -7469,7 +7475,7 @@
         <v>359</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="180">

</xml_diff>